<commit_message>
Mise à jour progression audit
</commit_message>
<xml_diff>
--- a/Audits/sommaireAudit2.xlsx
+++ b/Audits/sommaireAudit2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Combaxe\Audits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Combaxe\Combaxe_Utilities\Audits\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>No tâche</t>
   </si>
@@ -53,9 +53,6 @@
     <t>En cours</t>
   </si>
   <si>
-    <t>Attribué</t>
-  </si>
-  <si>
     <t>Fonctionnalité supprimer un personnage</t>
   </si>
   <si>
@@ -171,6 +168,18 @@
   </si>
   <si>
     <t>Faire fonctionner le chronomètre en combat</t>
+  </si>
+  <si>
+    <t>Fonctionnalité bouton fuir</t>
+  </si>
+  <si>
+    <t>La taverne</t>
+  </si>
+  <si>
+    <t>Fonctionnalité concernant le bouton qui permet de fuir</t>
+  </si>
+  <si>
+    <t>Faire la taverne qui regénère la vie</t>
   </si>
 </sst>
 </file>
@@ -236,7 +245,57 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -613,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,11 +712,11 @@
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -671,11 +730,11 @@
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
         <v>2.5</v>
@@ -689,11 +748,11 @@
         <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
@@ -707,11 +766,11 @@
         <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -730,10 +789,10 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>8</v>
@@ -744,13 +803,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2">
         <v>0.5</v>
@@ -759,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -767,13 +826,13 @@
         <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2">
         <v>10.5</v>
@@ -787,13 +846,13 @@
         <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="2">
         <v>0.5</v>
@@ -807,13 +866,13 @@
         <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2">
         <v>0.5</v>
@@ -827,13 +886,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2">
         <v>4</v>
@@ -847,13 +906,13 @@
         <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
@@ -867,13 +926,13 @@
         <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E13" s="2">
         <v>5.5</v>
@@ -887,19 +946,19 @@
         <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="2">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -907,19 +966,19 @@
         <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="2">
         <v>6</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -927,19 +986,19 @@
         <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="2">
         <v>6</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -947,19 +1006,19 @@
         <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="2">
         <v>6</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -967,19 +1026,19 @@
         <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" s="2">
         <v>6</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -987,11 +1046,11 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="2">
         <v>4</v>
@@ -1005,13 +1064,13 @@
         <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" s="2">
         <v>1</v>
@@ -1025,115 +1084,160 @@
         <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E21" s="2">
         <v>2</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="2">
+        <v>34</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E22" s="2">
-        <f t="array" ref="E22">SUM(E2:E20)</f>
-        <v>70</v>
-      </c>
-      <c r="F22" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="A23" s="2">
+        <v>35</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="array" ref="E24">SUM(E2:E20)</f>
+        <v>63.5</v>
+      </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
+      <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2 A3:F19 G7 G5">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Terminé">
+  <conditionalFormatting sqref="F2 G7 G5 A3:F19">
+    <cfRule type="containsText" dxfId="3" priority="10" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21:F23">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",F21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>